<commit_message>
update mô tả gì đó
</commit_message>
<xml_diff>
--- a/dimension.xlsx
+++ b/dimension.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MDS\2025 model\model_antibiotic\antibiotic_GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97073411-397A-4508-A653-3C0A3DFB2647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F2F287-B5A1-41FE-A76C-808800EAD3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{2CF9D3B3-B84B-4BD9-ABA6-50253CB4FDC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{2CF9D3B3-B84B-4BD9-ABA6-50253CB4FDC8}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
     <sheet name="department_ordered" sheetId="2" r:id="rId2"/>
-    <sheet name="order_owner" sheetId="3" r:id="rId3"/>
+    <sheet name="order_owner.1" sheetId="3" r:id="rId3"/>
+    <sheet name="specimen_source" sheetId="4" r:id="rId4"/>
+    <sheet name="organism" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="214">
   <si>
     <t>location</t>
   </si>
@@ -243,9 +245,6 @@
     <t>Dr. Le Minh Duc</t>
   </si>
   <si>
-    <t>Dr. Le Thanh Hai Dang</t>
-  </si>
-  <si>
     <t>Dr. Le Thi Bich Tram</t>
   </si>
   <si>
@@ -255,9 +254,6 @@
     <t>Dr. Ly Quoc Thinh</t>
   </si>
   <si>
-    <t>Dr. Ngo Trung Nam</t>
-  </si>
-  <si>
     <t>Dr. Ngo Viet Thang</t>
   </si>
   <si>
@@ -285,9 +281,6 @@
     <t>Dr. Nguyen Thi Lam Giang</t>
   </si>
   <si>
-    <t>Dr. Nguyen Thi Ngoc Dung</t>
-  </si>
-  <si>
     <t>Dr. Nguyen Thi Thu Huong</t>
   </si>
   <si>
@@ -300,9 +293,6 @@
     <t>Dr. Nguyen Van Quy</t>
   </si>
   <si>
-    <t>Dr. Pham Bich Chi</t>
-  </si>
-  <si>
     <t>Dr. Pham Dang Tinh</t>
   </si>
   <si>
@@ -312,21 +302,12 @@
     <t>Dr. Pham Thai Binh</t>
   </si>
   <si>
-    <t>Dr. Phan Thi Thanh Huyen</t>
-  </si>
-  <si>
     <t>Dr. Tran Nhu Tuong Van</t>
   </si>
   <si>
-    <t>Dr. Tran Pham Dieu</t>
-  </si>
-  <si>
     <t>Dr. Tran Thi Phuong Thao</t>
   </si>
   <si>
-    <t>Dr. Tran Trieu Phuong Dong</t>
-  </si>
-  <si>
     <t>Dr. Tran Xuan Tiem</t>
   </si>
   <si>
@@ -348,10 +329,358 @@
     <t>Dr. Vu Ngoc Chuc</t>
   </si>
   <si>
-    <t>Dr. Vuong Kim Dung</t>
-  </si>
-  <si>
     <t>department_ordered</t>
+  </si>
+  <si>
+    <t>Dr. Bernard COLIN</t>
+  </si>
+  <si>
+    <t>Dr. Bui Nhuan Quy</t>
+  </si>
+  <si>
+    <t>Dr. Lam Phuoc Loc</t>
+  </si>
+  <si>
+    <t>Dr. Le Duc Tuan</t>
+  </si>
+  <si>
+    <t>Dr. Le Nguyen Anh Thi</t>
+  </si>
+  <si>
+    <t>Dr. Le Trong Phat</t>
+  </si>
+  <si>
+    <t>Dr. Luong Ngoc Trung</t>
+  </si>
+  <si>
+    <t>Dr. Nguyen Thanh Vinh</t>
+  </si>
+  <si>
+    <t>Dr. Nguyen Thi Bay</t>
+  </si>
+  <si>
+    <t>Dr. Nguyen Thi Thanh Minh</t>
+  </si>
+  <si>
+    <t>Dr. Nguyen Tuan Dinh</t>
+  </si>
+  <si>
+    <t>Dr. Nguyen Van Tho</t>
+  </si>
+  <si>
+    <t>Dr. Pham Long Dao</t>
+  </si>
+  <si>
+    <t>Dr. Pham Nguyen Thanh Nam</t>
+  </si>
+  <si>
+    <t>Dr. Pham The Kien</t>
+  </si>
+  <si>
+    <t>Dr. Pham Tuan</t>
+  </si>
+  <si>
+    <t>Dr. Phan Van Thai</t>
+  </si>
+  <si>
+    <t>Dr. Trinh Van Hai</t>
+  </si>
+  <si>
+    <t>Dr. Truong My Hanh Tram</t>
+  </si>
+  <si>
+    <t>Dr. Vu Hoang Lien</t>
+  </si>
+  <si>
+    <t>Prof. Pham Trinh Quoc Khanh</t>
+  </si>
+  <si>
+    <t>Abdominal Fluid</t>
+  </si>
+  <si>
+    <t>Bile</t>
+  </si>
+  <si>
+    <t>Blood Cult. Aerobic</t>
+  </si>
+  <si>
+    <t>Blood Cult. Anaerobic</t>
+  </si>
+  <si>
+    <t>Blood Cult. Pediatric</t>
+  </si>
+  <si>
+    <t>Bron. Alv. Lav. (BAL)</t>
+  </si>
+  <si>
+    <t>Cath - Central</t>
+  </si>
+  <si>
+    <t>Cath - Peripheral</t>
+  </si>
+  <si>
+    <t>CSF</t>
+  </si>
+  <si>
+    <t>Fluid</t>
+  </si>
+  <si>
+    <t>Genital - Swab</t>
+  </si>
+  <si>
+    <t>Nasopharyngeal</t>
+  </si>
+  <si>
+    <t>Pul. Tracheal Aspiration</t>
+  </si>
+  <si>
+    <t>Puncture Fluid</t>
+  </si>
+  <si>
+    <t>Pus - Swab</t>
+  </si>
+  <si>
+    <t>Pus Fluid</t>
+  </si>
+  <si>
+    <t>Set 1 Aerobic Bottle</t>
+  </si>
+  <si>
+    <t>Set 1 Anaerobic Bottle</t>
+  </si>
+  <si>
+    <t>Set 2 Aerobic Bottle</t>
+  </si>
+  <si>
+    <t>Set 2 Anaerobic Bottle</t>
+  </si>
+  <si>
+    <t>Skin Lesion - Swab</t>
+  </si>
+  <si>
+    <t>Sputum</t>
+  </si>
+  <si>
+    <t>Stool</t>
+  </si>
+  <si>
+    <t>Throat</t>
+  </si>
+  <si>
+    <t>Urine Mid-Stream</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>ISOLATE_ORGANISM</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Haemophilus influenzae</t>
+  </si>
+  <si>
+    <t>Candida albicans</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Moraxella catarrhalis (Branhamella catarrhalis)</t>
+  </si>
+  <si>
+    <t>Klebsiella aerogenes</t>
+  </si>
+  <si>
+    <t>Gram-negative bacilli (identification in process)</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>Staphylococcus lugdunensis</t>
+  </si>
+  <si>
+    <t>Salmonella spp</t>
+  </si>
+  <si>
+    <t>Haemophilus parainfluenzae</t>
+  </si>
+  <si>
+    <t>Enterococcus faecium</t>
+  </si>
+  <si>
+    <t>Candida tropicalis</t>
+  </si>
+  <si>
+    <t>Streptococcus pyogenes (Streptococcus group A)</t>
+  </si>
+  <si>
+    <t>Serratia marcescens</t>
+  </si>
+  <si>
+    <t>Comamonas testosteroni</t>
+  </si>
+  <si>
+    <t>Enterococcus faecalis</t>
+  </si>
+  <si>
+    <t>Staphylococcus haemolyticus</t>
+  </si>
+  <si>
+    <t>Staphylococcus hominis</t>
+  </si>
+  <si>
+    <t>Acinetobacter baumannii</t>
+  </si>
+  <si>
+    <t>Klebsiella pneumoniae ssp pneumoniae</t>
+  </si>
+  <si>
+    <t>Proteus mirabilis</t>
+  </si>
+  <si>
+    <t>Streptococcus agalactiae</t>
+  </si>
+  <si>
+    <t>Providencia rettgeri</t>
+  </si>
+  <si>
+    <t>Candida glabrata</t>
+  </si>
+  <si>
+    <t>Stenotrophomonas maltophilia</t>
+  </si>
+  <si>
+    <t>Staphylococcus epidermidis</t>
+  </si>
+  <si>
+    <t>Enterobacter cloacae</t>
+  </si>
+  <si>
+    <t>Pantoea sp</t>
+  </si>
+  <si>
+    <t>Streptococcus pneumoniae</t>
+  </si>
+  <si>
+    <t>Staphylococcus sciuri</t>
+  </si>
+  <si>
+    <t>Enterococcus gallinarum</t>
+  </si>
+  <si>
+    <t>Enterobacter cloacae complex</t>
+  </si>
+  <si>
+    <t>Lactobacillus salivarius</t>
+  </si>
+  <si>
+    <t>Citrobacter freundii</t>
+  </si>
+  <si>
+    <t>Proteus vulgaris</t>
+  </si>
+  <si>
+    <t>Proteus penneri</t>
+  </si>
+  <si>
+    <t>Morganella morganii</t>
+  </si>
+  <si>
+    <t>Corynebacterium striatum</t>
+  </si>
+  <si>
+    <t>Candida dubliniensis</t>
+  </si>
+  <si>
+    <t>Citrobacter koserii</t>
+  </si>
+  <si>
+    <t>Streptococcus constellatus</t>
+  </si>
+  <si>
+    <t>Candida krusei</t>
+  </si>
+  <si>
+    <t>Enterococcus casseliflavus</t>
+  </si>
+  <si>
+    <t>Streptococcus gallolyticus ssp gallolyticus</t>
+  </si>
+  <si>
+    <t>Corynebacterium sp</t>
+  </si>
+  <si>
+    <t>Providencia stuartii</t>
+  </si>
+  <si>
+    <t>Enterococcus avium</t>
+  </si>
+  <si>
+    <t>Achromobacter denitrificans</t>
+  </si>
+  <si>
+    <t>Streptococcus group B</t>
+  </si>
+  <si>
+    <t>Streptococcus gallolyticus ssp pasteurianus</t>
+  </si>
+  <si>
+    <t>Acinetobacter baumannii complex</t>
+  </si>
+  <si>
+    <t>Kluyvera cryocrescens</t>
+  </si>
+  <si>
+    <t>Streptococcus pyogenes</t>
+  </si>
+  <si>
+    <t>Burkholderia cepacia</t>
+  </si>
+  <si>
+    <t>Pseudomonas stutzeri</t>
+  </si>
+  <si>
+    <t>Candida parapsilosis</t>
+  </si>
+  <si>
+    <t>Streptococcus intermedius</t>
+  </si>
+  <si>
+    <t>Aeromonas hydrophila/punctata(caviae)</t>
+  </si>
+  <si>
+    <t>Coagulase negative Staphylococcus</t>
+  </si>
+  <si>
+    <t>Edwardsiella tarda</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii</t>
+  </si>
+  <si>
+    <t>Burkholderia gladioli</t>
+  </si>
+  <si>
+    <t>Bacillus cereus group</t>
+  </si>
+  <si>
+    <t>Klebsiella oxytoca</t>
+  </si>
+  <si>
+    <t>Pantoea dispersa</t>
+  </si>
+  <si>
+    <t>Pseudomonas mendocina</t>
+  </si>
+  <si>
+    <t>Citrobacter amalonaticus</t>
   </si>
 </sst>
 </file>
@@ -801,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE525E3B-B6E7-489D-A229-CE3D8D6EB7CF}">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1032,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131E4C92-E903-49C5-8B2E-3565B11A3BAA}">
-  <dimension ref="A1:A55"/>
+  <dimension ref="A1:A68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,270 +1384,853 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9C7BD7-9843-4113-A107-B4A5F34E8E8C}">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FA9CEA-2DD7-4D36-9E86-FFAF6FA84002}">
+  <dimension ref="A1:A70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A70">
+    <sortCondition ref="A2:A70"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>